<commit_message>
search with thranslation. reworked custom filter
</commit_message>
<xml_diff>
--- a/export/Export 2020!04!19(18!18).xlsx
+++ b/export/Export 2020!04!19(18!18).xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liffex\Desktop\Diplom\Test diplom\export\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист 1" r:id="rId3" sheetId="1"/>
+    <sheet name="Лист 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9072" uniqueCount="959">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4329" uniqueCount="960">
   <si>
     <t/>
   </si>
@@ -2889,16 +2896,18 @@
   </si>
   <si>
     <t>война</t>
+  </si>
+  <si>
+    <t>Политика</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2910,7 +2919,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -2928,18 +2937,294 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+  <a:themeElements>
+    <a:clrScheme name="Стандартная">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Стандартная">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Стандартная">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K432"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L432"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L31" sqref="A23:L31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2974,7 +3259,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3009,7 +3294,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3044,7 +3329,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -3079,7 +3364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -3114,7 +3399,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -3149,7 +3434,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -3184,7 +3469,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -3219,7 +3504,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -3254,7 +3539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -3289,7 +3574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -3324,7 +3609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -3359,7 +3644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -3394,7 +3679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -3429,7 +3714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -3464,7 +3749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -3499,7 +3784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -3534,7 +3819,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -3569,7 +3854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -3604,7 +3889,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -3639,7 +3924,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -3674,7 +3959,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -3709,7 +3994,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -3743,8 +4028,11 @@
       <c r="K23" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24">
+      <c r="L23" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>73</v>
       </c>
@@ -3778,8 +4066,11 @@
       <c r="K24" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="25">
+      <c r="L24" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -3813,8 +4104,11 @@
       <c r="K25" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="26">
+      <c r="L25" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -3848,8 +4142,11 @@
       <c r="K26" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27">
+      <c r="L26" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -3883,8 +4180,11 @@
       <c r="K27" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="28">
+      <c r="L27" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>86</v>
       </c>
@@ -3918,8 +4218,11 @@
       <c r="K28" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="29">
+      <c r="L28" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -3953,8 +4256,11 @@
       <c r="K29" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="30">
+      <c r="L29" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>94</v>
       </c>
@@ -3988,8 +4294,11 @@
       <c r="K30" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="31">
+      <c r="L30" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>97</v>
       </c>
@@ -4023,8 +4332,11 @@
       <c r="K31" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="32">
+      <c r="L31" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>97</v>
       </c>
@@ -4059,7 +4371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -4094,7 +4406,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>97</v>
       </c>
@@ -4129,7 +4441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -4164,7 +4476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>97</v>
       </c>
@@ -4199,7 +4511,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -4234,7 +4546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -4269,7 +4581,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>97</v>
       </c>
@@ -4304,7 +4616,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -4339,7 +4651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>97</v>
       </c>
@@ -4374,7 +4686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>120</v>
       </c>
@@ -4409,7 +4721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>120</v>
       </c>
@@ -4444,7 +4756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>124</v>
       </c>
@@ -4479,7 +4791,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>124</v>
       </c>
@@ -4514,7 +4826,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>130</v>
       </c>
@@ -4549,7 +4861,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>130</v>
       </c>
@@ -4584,7 +4896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>130</v>
       </c>
@@ -4619,7 +4931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>130</v>
       </c>
@@ -4654,7 +4966,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>130</v>
       </c>
@@ -4689,7 +5001,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>141</v>
       </c>
@@ -4724,7 +5036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>145</v>
       </c>
@@ -4759,7 +5071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>145</v>
       </c>
@@ -4794,7 +5106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>145</v>
       </c>
@@ -4829,7 +5141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>145</v>
       </c>
@@ -4864,7 +5176,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>145</v>
       </c>
@@ -4899,7 +5211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>154</v>
       </c>
@@ -4934,7 +5246,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>158</v>
       </c>
@@ -4969,7 +5281,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>158</v>
       </c>
@@ -5004,7 +5316,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>158</v>
       </c>
@@ -5039,7 +5351,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>158</v>
       </c>
@@ -5074,7 +5386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>158</v>
       </c>
@@ -5109,7 +5421,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>158</v>
       </c>
@@ -5144,7 +5456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>172</v>
       </c>
@@ -5179,7 +5491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>175</v>
       </c>
@@ -5214,7 +5526,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>175</v>
       </c>
@@ -5249,7 +5561,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>175</v>
       </c>
@@ -5284,7 +5596,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>182</v>
       </c>
@@ -5319,7 +5631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>185</v>
       </c>
@@ -5354,7 +5666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>185</v>
       </c>
@@ -5389,7 +5701,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>185</v>
       </c>
@@ -5424,7 +5736,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>191</v>
       </c>
@@ -5459,7 +5771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>191</v>
       </c>
@@ -5494,7 +5806,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>191</v>
       </c>
@@ -5529,7 +5841,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>199</v>
       </c>
@@ -5564,7 +5876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>203</v>
       </c>
@@ -5599,7 +5911,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>206</v>
       </c>
@@ -5634,7 +5946,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>206</v>
       </c>
@@ -5669,7 +5981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>206</v>
       </c>
@@ -5704,7 +6016,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>206</v>
       </c>
@@ -5739,7 +6051,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>206</v>
       </c>
@@ -5774,7 +6086,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>206</v>
       </c>
@@ -5809,7 +6121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>206</v>
       </c>
@@ -5844,7 +6156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>206</v>
       </c>
@@ -5879,7 +6191,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>206</v>
       </c>
@@ -5914,7 +6226,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>234</v>
       </c>
@@ -5949,7 +6261,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>234</v>
       </c>
@@ -5984,7 +6296,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>239</v>
       </c>
@@ -6019,7 +6331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>241</v>
       </c>
@@ -6054,7 +6366,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>244</v>
       </c>
@@ -6089,7 +6401,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>247</v>
       </c>
@@ -6124,7 +6436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>251</v>
       </c>
@@ -6159,7 +6471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>251</v>
       </c>
@@ -6194,7 +6506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>257</v>
       </c>
@@ -6229,7 +6541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>260</v>
       </c>
@@ -6264,7 +6576,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>263</v>
       </c>
@@ -6299,7 +6611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>267</v>
       </c>
@@ -6334,7 +6646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>269</v>
       </c>
@@ -6369,7 +6681,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>269</v>
       </c>
@@ -6404,7 +6716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>269</v>
       </c>
@@ -6439,7 +6751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>269</v>
       </c>
@@ -6474,7 +6786,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>269</v>
       </c>
@@ -6509,7 +6821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>269</v>
       </c>
@@ -6544,7 +6856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>269</v>
       </c>
@@ -6579,7 +6891,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>289</v>
       </c>
@@ -6614,7 +6926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>276</v>
       </c>
@@ -6649,7 +6961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>276</v>
       </c>
@@ -6684,7 +6996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>276</v>
       </c>
@@ -6719,7 +7031,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>301</v>
       </c>
@@ -6754,7 +7066,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>304</v>
       </c>
@@ -6789,7 +7101,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>306</v>
       </c>
@@ -6824,7 +7136,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>310</v>
       </c>
@@ -6859,7 +7171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>311</v>
       </c>
@@ -6894,7 +7206,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>314</v>
       </c>
@@ -6929,7 +7241,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>314</v>
       </c>
@@ -6964,7 +7276,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>314</v>
       </c>
@@ -6999,7 +7311,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>314</v>
       </c>
@@ -7034,7 +7346,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>321</v>
       </c>
@@ -7069,7 +7381,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>322</v>
       </c>
@@ -7104,7 +7416,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>325</v>
       </c>
@@ -7139,7 +7451,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>325</v>
       </c>
@@ -7174,7 +7486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>330</v>
       </c>
@@ -7209,7 +7521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>330</v>
       </c>
@@ -7244,7 +7556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>330</v>
       </c>
@@ -7279,7 +7591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>330</v>
       </c>
@@ -7314,7 +7626,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>330</v>
       </c>
@@ -7349,7 +7661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>344</v>
       </c>
@@ -7384,7 +7696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>347</v>
       </c>
@@ -7419,7 +7731,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>347</v>
       </c>
@@ -7454,7 +7766,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>347</v>
       </c>
@@ -7489,7 +7801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>354</v>
       </c>
@@ -7524,7 +7836,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>358</v>
       </c>
@@ -7559,7 +7871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>358</v>
       </c>
@@ -7594,7 +7906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>364</v>
       </c>
@@ -7629,7 +7941,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>368</v>
       </c>
@@ -7664,7 +7976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>371</v>
       </c>
@@ -7699,7 +8011,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>375</v>
       </c>
@@ -7734,7 +8046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>376</v>
       </c>
@@ -7769,7 +8081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>378</v>
       </c>
@@ -7804,7 +8116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>381</v>
       </c>
@@ -7839,7 +8151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>382</v>
       </c>
@@ -7874,7 +8186,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>386</v>
       </c>
@@ -7909,7 +8221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>387</v>
       </c>
@@ -7944,7 +8256,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>391</v>
       </c>
@@ -7979,7 +8291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>394</v>
       </c>
@@ -8014,7 +8326,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>394</v>
       </c>
@@ -8049,7 +8361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>394</v>
       </c>
@@ -8084,7 +8396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>394</v>
       </c>
@@ -8119,7 +8431,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>394</v>
       </c>
@@ -8154,7 +8466,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>394</v>
       </c>
@@ -8189,7 +8501,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>394</v>
       </c>
@@ -8224,7 +8536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>394</v>
       </c>
@@ -8259,7 +8571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>394</v>
       </c>
@@ -8294,7 +8606,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>409</v>
       </c>
@@ -8329,7 +8641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>411</v>
       </c>
@@ -8364,7 +8676,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>414</v>
       </c>
@@ -8399,7 +8711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>414</v>
       </c>
@@ -8434,7 +8746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>414</v>
       </c>
@@ -8469,7 +8781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>414</v>
       </c>
@@ -8504,7 +8816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>414</v>
       </c>
@@ -8539,7 +8851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>414</v>
       </c>
@@ -8574,7 +8886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>414</v>
       </c>
@@ -8609,7 +8921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>414</v>
       </c>
@@ -8644,7 +8956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>414</v>
       </c>
@@ -8679,7 +8991,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>414</v>
       </c>
@@ -8714,7 +9026,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>431</v>
       </c>
@@ -8749,7 +9061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>434</v>
       </c>
@@ -8784,7 +9096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>438</v>
       </c>
@@ -8819,7 +9131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>438</v>
       </c>
@@ -8854,7 +9166,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>444</v>
       </c>
@@ -8889,7 +9201,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>447</v>
       </c>
@@ -8924,7 +9236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>447</v>
       </c>
@@ -8959,7 +9271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>447</v>
       </c>
@@ -8994,7 +9306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>447</v>
       </c>
@@ -9029,7 +9341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>447</v>
       </c>
@@ -9064,7 +9376,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>458</v>
       </c>
@@ -9099,7 +9411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>458</v>
       </c>
@@ -9134,7 +9446,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>458</v>
       </c>
@@ -9169,7 +9481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>458</v>
       </c>
@@ -9204,7 +9516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>458</v>
       </c>
@@ -9239,7 +9551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>458</v>
       </c>
@@ -9274,7 +9586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>458</v>
       </c>
@@ -9309,7 +9621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>458</v>
       </c>
@@ -9344,7 +9656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>458</v>
       </c>
@@ -9379,7 +9691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>458</v>
       </c>
@@ -9414,7 +9726,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>458</v>
       </c>
@@ -9449,7 +9761,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>458</v>
       </c>
@@ -9484,7 +9796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>458</v>
       </c>
@@ -9519,7 +9831,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>458</v>
       </c>
@@ -9554,7 +9866,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>458</v>
       </c>
@@ -9589,7 +9901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>458</v>
       </c>
@@ -9624,7 +9936,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>458</v>
       </c>
@@ -9659,7 +9971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>458</v>
       </c>
@@ -9694,7 +10006,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>458</v>
       </c>
@@ -9729,7 +10041,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>458</v>
       </c>
@@ -9764,7 +10076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>494</v>
       </c>
@@ -9799,7 +10111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>497</v>
       </c>
@@ -9834,7 +10146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>498</v>
       </c>
@@ -9869,7 +10181,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>499</v>
       </c>
@@ -9904,7 +10216,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>502</v>
       </c>
@@ -9939,7 +10251,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>503</v>
       </c>
@@ -9974,7 +10286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="202">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>506</v>
       </c>
@@ -10009,7 +10321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>506</v>
       </c>
@@ -10044,7 +10356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>511</v>
       </c>
@@ -10079,7 +10391,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="205">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>511</v>
       </c>
@@ -10114,7 +10426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="206">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>516</v>
       </c>
@@ -10149,7 +10461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="207">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>516</v>
       </c>
@@ -10184,7 +10496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="208">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>516</v>
       </c>
@@ -10219,7 +10531,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="209">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>516</v>
       </c>
@@ -10254,7 +10566,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="210">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>516</v>
       </c>
@@ -10289,7 +10601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="211">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>516</v>
       </c>
@@ -10324,7 +10636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="212">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>530</v>
       </c>
@@ -10359,7 +10671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>534</v>
       </c>
@@ -10394,7 +10706,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>536</v>
       </c>
@@ -10429,7 +10741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="215">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>539</v>
       </c>
@@ -10464,7 +10776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="216">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>539</v>
       </c>
@@ -10499,7 +10811,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="217">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>539</v>
       </c>
@@ -10534,7 +10846,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="218">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>539</v>
       </c>
@@ -10569,7 +10881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="219">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>539</v>
       </c>
@@ -10604,7 +10916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="220">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>539</v>
       </c>
@@ -10639,7 +10951,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="221">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>539</v>
       </c>
@@ -10674,7 +10986,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="222">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>539</v>
       </c>
@@ -10709,7 +11021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="223">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>539</v>
       </c>
@@ -10744,7 +11056,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="224">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>539</v>
       </c>
@@ -10779,7 +11091,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="225">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>539</v>
       </c>
@@ -10814,7 +11126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="226">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>554</v>
       </c>
@@ -10849,7 +11161,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="227">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>557</v>
       </c>
@@ -10884,7 +11196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="228">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>559</v>
       </c>
@@ -10919,7 +11231,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="229">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>562</v>
       </c>
@@ -10954,7 +11266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="230">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>565</v>
       </c>
@@ -10989,7 +11301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="231">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>569</v>
       </c>
@@ -11024,7 +11336,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="232">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>573</v>
       </c>
@@ -11059,7 +11371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="233">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>573</v>
       </c>
@@ -11094,7 +11406,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="234">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>573</v>
       </c>
@@ -11129,7 +11441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="235">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>573</v>
       </c>
@@ -11164,7 +11476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="236">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>573</v>
       </c>
@@ -11199,7 +11511,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="237">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>573</v>
       </c>
@@ -11234,7 +11546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="238">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>573</v>
       </c>
@@ -11269,7 +11581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="239">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>573</v>
       </c>
@@ -11304,7 +11616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="240">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>594</v>
       </c>
@@ -11339,7 +11651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="241">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>595</v>
       </c>
@@ -11374,7 +11686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="242">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>595</v>
       </c>
@@ -11409,7 +11721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="243">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>598</v>
       </c>
@@ -11444,7 +11756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="244">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>598</v>
       </c>
@@ -11479,7 +11791,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="245">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>598</v>
       </c>
@@ -11514,7 +11826,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="246">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>598</v>
       </c>
@@ -11549,7 +11861,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="247">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>608</v>
       </c>
@@ -11584,7 +11896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="248">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>608</v>
       </c>
@@ -11619,7 +11931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="249">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>608</v>
       </c>
@@ -11654,7 +11966,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="250">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>617</v>
       </c>
@@ -11689,7 +12001,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="251">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>618</v>
       </c>
@@ -11724,7 +12036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="252">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>622</v>
       </c>
@@ -11759,7 +12071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="253">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>624</v>
       </c>
@@ -11794,7 +12106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="254">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>624</v>
       </c>
@@ -11829,7 +12141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="255">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>631</v>
       </c>
@@ -11864,7 +12176,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="256">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>632</v>
       </c>
@@ -11899,7 +12211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="257">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>635</v>
       </c>
@@ -11934,7 +12246,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="258">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>635</v>
       </c>
@@ -11969,7 +12281,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="259">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>635</v>
       </c>
@@ -12004,7 +12316,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="260">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>635</v>
       </c>
@@ -12039,7 +12351,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="261">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>635</v>
       </c>
@@ -12074,7 +12386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="262">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>635</v>
       </c>
@@ -12109,7 +12421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="263">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>635</v>
       </c>
@@ -12144,7 +12456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="264">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>635</v>
       </c>
@@ -12179,7 +12491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="265">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>635</v>
       </c>
@@ -12214,7 +12526,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="266">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>635</v>
       </c>
@@ -12249,7 +12561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="267">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>635</v>
       </c>
@@ -12284,7 +12596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="268">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>635</v>
       </c>
@@ -12319,7 +12631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="269">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>635</v>
       </c>
@@ -12354,7 +12666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="270">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>635</v>
       </c>
@@ -12389,7 +12701,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="271">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>635</v>
       </c>
@@ -12424,7 +12736,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="272">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>635</v>
       </c>
@@ -12459,7 +12771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="273">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>635</v>
       </c>
@@ -12494,7 +12806,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="274">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>635</v>
       </c>
@@ -12529,7 +12841,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="275">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>635</v>
       </c>
@@ -12564,7 +12876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="276">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>635</v>
       </c>
@@ -12599,7 +12911,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="277">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>635</v>
       </c>
@@ -12634,7 +12946,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="278">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>635</v>
       </c>
@@ -12669,7 +12981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="279">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>635</v>
       </c>
@@ -12704,7 +13016,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="280">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>635</v>
       </c>
@@ -12739,7 +13051,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="281">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>635</v>
       </c>
@@ -12774,7 +13086,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="282">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>635</v>
       </c>
@@ -12809,7 +13121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="283">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>635</v>
       </c>
@@ -12844,7 +13156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="284">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>635</v>
       </c>
@@ -12879,7 +13191,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="285">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>635</v>
       </c>
@@ -12914,7 +13226,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="286">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>635</v>
       </c>
@@ -12949,7 +13261,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="287">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>635</v>
       </c>
@@ -12984,7 +13296,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="288">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>635</v>
       </c>
@@ -13019,7 +13331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="289">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>680</v>
       </c>
@@ -13054,7 +13366,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="290">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>683</v>
       </c>
@@ -13089,7 +13401,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="291">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>686</v>
       </c>
@@ -13124,7 +13436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="292">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>686</v>
       </c>
@@ -13159,7 +13471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="293">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>692</v>
       </c>
@@ -13194,7 +13506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="294">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>693</v>
       </c>
@@ -13229,7 +13541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="295">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>695</v>
       </c>
@@ -13264,7 +13576,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="296">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>698</v>
       </c>
@@ -13299,7 +13611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="297">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>701</v>
       </c>
@@ -13334,7 +13646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="298">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>701</v>
       </c>
@@ -13369,7 +13681,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="299">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>701</v>
       </c>
@@ -13404,7 +13716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="300">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>701</v>
       </c>
@@ -13439,7 +13751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="301">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>709</v>
       </c>
@@ -13474,7 +13786,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="302">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>712</v>
       </c>
@@ -13509,7 +13821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="303">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>715</v>
       </c>
@@ -13544,7 +13856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="304">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>715</v>
       </c>
@@ -13579,7 +13891,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="305">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>715</v>
       </c>
@@ -13614,7 +13926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="306">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>715</v>
       </c>
@@ -13649,7 +13961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="307">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>718</v>
       </c>
@@ -13684,7 +13996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="308">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>718</v>
       </c>
@@ -13719,7 +14031,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="309">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>719</v>
       </c>
@@ -13754,7 +14066,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="310">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>722</v>
       </c>
@@ -13789,7 +14101,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="311">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>726</v>
       </c>
@@ -13824,7 +14136,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="312">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>729</v>
       </c>
@@ -13859,7 +14171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="313">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>733</v>
       </c>
@@ -13894,7 +14206,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="314">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>736</v>
       </c>
@@ -13929,7 +14241,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="315">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>736</v>
       </c>
@@ -13964,7 +14276,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="316">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>736</v>
       </c>
@@ -13999,7 +14311,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="317">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>736</v>
       </c>
@@ -14034,7 +14346,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="318">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>745</v>
       </c>
@@ -14069,7 +14381,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="319">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>748</v>
       </c>
@@ -14104,7 +14416,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="320">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>750</v>
       </c>
@@ -14139,7 +14451,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="321">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>752</v>
       </c>
@@ -14174,7 +14486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="322">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>755</v>
       </c>
@@ -14209,7 +14521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="323">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>755</v>
       </c>
@@ -14244,7 +14556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="324">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>755</v>
       </c>
@@ -14279,7 +14591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="325">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>755</v>
       </c>
@@ -14314,7 +14626,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="326">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>755</v>
       </c>
@@ -14349,7 +14661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="327">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>763</v>
       </c>
@@ -14384,7 +14696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="328">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>763</v>
       </c>
@@ -14419,7 +14731,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="329">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>770</v>
       </c>
@@ -14454,7 +14766,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="330">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>772</v>
       </c>
@@ -14489,7 +14801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="331">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>776</v>
       </c>
@@ -14524,7 +14836,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="332">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>776</v>
       </c>
@@ -14559,7 +14871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="333">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>776</v>
       </c>
@@ -14594,7 +14906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="334">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>782</v>
       </c>
@@ -14629,7 +14941,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="335">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>784</v>
       </c>
@@ -14664,7 +14976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="336">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>787</v>
       </c>
@@ -14699,7 +15011,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="337">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>790</v>
       </c>
@@ -14734,7 +15046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="338">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>790</v>
       </c>
@@ -14769,7 +15081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="339">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>790</v>
       </c>
@@ -14804,7 +15116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="340">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>793</v>
       </c>
@@ -14839,7 +15151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="341">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>793</v>
       </c>
@@ -14874,7 +15186,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="342">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>793</v>
       </c>
@@ -14909,7 +15221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="343">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>793</v>
       </c>
@@ -14944,7 +15256,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="344">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>793</v>
       </c>
@@ -14979,7 +15291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="345">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>793</v>
       </c>
@@ -15014,7 +15326,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="346">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>793</v>
       </c>
@@ -15049,7 +15361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="347">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>793</v>
       </c>
@@ -15084,7 +15396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="348">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>793</v>
       </c>
@@ -15119,7 +15431,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="349">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>793</v>
       </c>
@@ -15154,7 +15466,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="350">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>793</v>
       </c>
@@ -15189,7 +15501,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="351">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>793</v>
       </c>
@@ -15224,7 +15536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="352">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>793</v>
       </c>
@@ -15259,7 +15571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="353">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>793</v>
       </c>
@@ -15294,7 +15606,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="354">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>793</v>
       </c>
@@ -15329,7 +15641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="355">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>793</v>
       </c>
@@ -15364,7 +15676,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="356">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>793</v>
       </c>
@@ -15399,7 +15711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="357">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>793</v>
       </c>
@@ -15434,7 +15746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="358">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>816</v>
       </c>
@@ -15469,7 +15781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="359">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>816</v>
       </c>
@@ -15504,7 +15816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="360">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>816</v>
       </c>
@@ -15539,7 +15851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="361">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>823</v>
       </c>
@@ -15574,7 +15886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="362">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>824</v>
       </c>
@@ -15609,7 +15921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="363">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>827</v>
       </c>
@@ -15644,7 +15956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="364">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>827</v>
       </c>
@@ -15679,7 +15991,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="365">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>832</v>
       </c>
@@ -15714,7 +16026,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="366">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>834</v>
       </c>
@@ -15749,7 +16061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="367">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>834</v>
       </c>
@@ -15784,7 +16096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="368">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>834</v>
       </c>
@@ -15819,7 +16131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="369">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>837</v>
       </c>
@@ -15854,7 +16166,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="370">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>838</v>
       </c>
@@ -15889,7 +16201,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="371">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>838</v>
       </c>
@@ -15924,7 +16236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="372">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>838</v>
       </c>
@@ -15959,7 +16271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="373">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>844</v>
       </c>
@@ -15994,7 +16306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="374">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>844</v>
       </c>
@@ -16029,7 +16341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="375">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>844</v>
       </c>
@@ -16064,7 +16376,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="376">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>844</v>
       </c>
@@ -16099,7 +16411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="377">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>844</v>
       </c>
@@ -16134,7 +16446,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="378">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>850</v>
       </c>
@@ -16169,7 +16481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="379">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>850</v>
       </c>
@@ -16204,7 +16516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="380">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>850</v>
       </c>
@@ -16239,7 +16551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="381">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>850</v>
       </c>
@@ -16274,7 +16586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="382">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>850</v>
       </c>
@@ -16309,7 +16621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="383">
+    <row r="383" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>850</v>
       </c>
@@ -16344,7 +16656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="384">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>850</v>
       </c>
@@ -16379,7 +16691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="385">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>850</v>
       </c>
@@ -16414,7 +16726,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="386">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
         <v>850</v>
       </c>
@@ -16449,7 +16761,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="387">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
         <v>850</v>
       </c>
@@ -16484,7 +16796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="388">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
         <v>872</v>
       </c>
@@ -16519,7 +16831,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="389">
+    <row r="389" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
         <v>874</v>
       </c>
@@ -16554,7 +16866,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="390">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
         <v>877</v>
       </c>
@@ -16589,7 +16901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="391">
+    <row r="391" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
         <v>879</v>
       </c>
@@ -16624,7 +16936,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="392">
+    <row r="392" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>883</v>
       </c>
@@ -16659,7 +16971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="393">
+    <row r="393" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>886</v>
       </c>
@@ -16694,7 +17006,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="394">
+    <row r="394" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>889</v>
       </c>
@@ -16729,7 +17041,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="395">
+    <row r="395" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>892</v>
       </c>
@@ -16764,7 +17076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="396">
+    <row r="396" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>892</v>
       </c>
@@ -16799,7 +17111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="397">
+    <row r="397" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>892</v>
       </c>
@@ -16834,7 +17146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="398">
+    <row r="398" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
         <v>892</v>
       </c>
@@ -16869,7 +17181,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="399">
+    <row r="399" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>896</v>
       </c>
@@ -16904,7 +17216,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="400">
+    <row r="400" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>899</v>
       </c>
@@ -16939,7 +17251,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="401">
+    <row r="401" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>901</v>
       </c>
@@ -16974,7 +17286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="402">
+    <row r="402" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>901</v>
       </c>
@@ -17009,7 +17321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="403">
+    <row r="403" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>901</v>
       </c>
@@ -17044,7 +17356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="404">
+    <row r="404" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>901</v>
       </c>
@@ -17079,7 +17391,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="405">
+    <row r="405" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>901</v>
       </c>
@@ -17114,7 +17426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="406">
+    <row r="406" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>909</v>
       </c>
@@ -17149,7 +17461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="407">
+    <row r="407" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
         <v>910</v>
       </c>
@@ -17184,7 +17496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="408">
+    <row r="408" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
         <v>913</v>
       </c>
@@ -17219,7 +17531,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="409">
+    <row r="409" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>913</v>
       </c>
@@ -17254,7 +17566,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="410">
+    <row r="410" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>913</v>
       </c>
@@ -17289,7 +17601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="411">
+    <row r="411" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>913</v>
       </c>
@@ -17324,7 +17636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="412">
+    <row r="412" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
         <v>918</v>
       </c>
@@ -17359,7 +17671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="413">
+    <row r="413" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
         <v>919</v>
       </c>
@@ -17394,7 +17706,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="414">
+    <row r="414" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
         <v>920</v>
       </c>
@@ -17429,7 +17741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="415">
+    <row r="415" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
         <v>922</v>
       </c>
@@ -17464,7 +17776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="416">
+    <row r="416" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
         <v>924</v>
       </c>
@@ -17499,7 +17811,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="417">
+    <row r="417" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>926</v>
       </c>
@@ -17534,7 +17846,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="418">
+    <row r="418" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
         <v>927</v>
       </c>
@@ -17569,7 +17881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="419">
+    <row r="419" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
         <v>930</v>
       </c>
@@ -17604,7 +17916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="420">
+    <row r="420" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
         <v>933</v>
       </c>
@@ -17639,7 +17951,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="421">
+    <row r="421" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
         <v>936</v>
       </c>
@@ -17674,7 +17986,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="422">
+    <row r="422" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
         <v>937</v>
       </c>
@@ -17709,7 +18021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="423">
+    <row r="423" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
         <v>937</v>
       </c>
@@ -17744,7 +18056,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="424">
+    <row r="424" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A424" t="s">
         <v>1</v>
       </c>
@@ -17779,7 +18091,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="425">
+    <row r="425" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
         <v>1</v>
       </c>
@@ -17814,7 +18126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="426">
+    <row r="426" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
         <v>1</v>
       </c>
@@ -17849,7 +18161,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="427">
+    <row r="427" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
         <v>1</v>
       </c>
@@ -17884,7 +18196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="428">
+    <row r="428" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
         <v>1</v>
       </c>
@@ -17919,7 +18231,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="429">
+    <row r="429" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
         <v>951</v>
       </c>
@@ -17954,7 +18266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="430">
+    <row r="430" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
         <v>952</v>
       </c>
@@ -17989,7 +18301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="431">
+    <row r="431" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
         <v>955</v>
       </c>
@@ -18024,7 +18336,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="432">
+    <row r="432" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A432" t="s">
         <v>956</v>
       </c>
@@ -18060,6 +18372,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>